<commit_message>
table module options check
</commit_message>
<xml_diff>
--- a/cases/3-mixed-modules/src/xlsx.xlsx
+++ b/cases/3-mixed-modules/src/xlsx.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2883069F-2D37-4908-9160-DAA4F7885AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="one" sheetId="1" r:id="rId1"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
   <si>
     <t>on</t>
   </si>
@@ -51,12 +52,21 @@
   </si>
   <si>
     <t>y2</t>
+  </si>
+  <si>
+    <t>action</t>
+  </si>
+  <si>
+    <t>hasMeta</t>
+  </si>
+  <si>
+    <t>xxx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -116,7 +126,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -124,14 +134,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -169,7 +182,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -241,7 +254,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -414,16 +427,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -439,9 +452,12 @@
       <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -458,7 +474,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0</v>
       </c>
@@ -473,6 +489,22 @@
       </c>
       <c r="E6" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -482,16 +514,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -507,15 +539,18 @@
       <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -532,7 +567,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0</v>
       </c>
@@ -547,6 +582,14 @@
       </c>
       <c r="E6" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>